<commit_message>
Added inspector coverage constraints. Added avoidance_list file.
</commit_message>
<xml_diff>
--- a/data/base_aircraft_schedule.xlsx
+++ b/data/base_aircraft_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ohi-my.sharepoint.com/personal/eduardo_sulz_ohi_pt/Documents/Documents/Projects/Git Pessoal/mechanics-roster-optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{7B98ACF5-C9F1-48E7-ACD0-691BE34E0641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83FA51D-A831-42B6-A952-93A8DF00BDF5}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{7B98ACF5-C9F1-48E7-ACD0-691BE34E0641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F81083-0456-4BE6-97F8-1E7DBB77DDC3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5FBD7B1F-887B-49B6-BADE-D9F46FF9879F}"/>
   </bookViews>
@@ -459,10 +459,27 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -532,7 +549,7 @@
       </c>
       <c r="G2">
         <f ca="1">IF(B2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f ca="1">IF(B2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
@@ -544,7 +561,7 @@
       </c>
       <c r="J2">
         <f ca="1">IF(C2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <f ca="1">IF(C2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
@@ -552,7 +569,7 @@
       </c>
       <c r="L2">
         <f ca="1">IF(C2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f ca="1">IF(D2=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
@@ -587,39 +604,39 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G13" ca="1" si="0">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>0</v>
+        <f t="shared" ref="G3:G12" ca="1" si="0">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H13" ca="1" si="1">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <f t="shared" ref="H3:H12" ca="1" si="1">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" ca="1" si="2">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <f t="shared" ref="I3:I12" ca="1" si="2">IF(B3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J13" ca="1" si="3">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <f t="shared" ref="J3:J12" ca="1" si="3">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K13" ca="1" si="4">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>0</v>
+        <f t="shared" ref="K3:K12" ca="1" si="4">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <v>1</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L13" ca="1" si="5">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <f t="shared" ref="L3:L12" ca="1" si="5">IF(C3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M13" ca="1" si="6">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <f t="shared" ref="M3:M12" ca="1" si="6">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N13" ca="1" si="7">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <f t="shared" ref="N3:N12" ca="1" si="7">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O13" ca="1" si="8">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
+        <f t="shared" ref="O3:O12" ca="1" si="8">IF(D3=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -644,7 +661,7 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -656,7 +673,7 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
@@ -664,7 +681,7 @@
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="6"/>
@@ -708,7 +725,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="3"/>
@@ -716,7 +733,7 @@
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="5"/>
@@ -836,7 +853,7 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="7"/>
@@ -844,7 +861,7 @@
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -880,7 +897,7 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
@@ -892,11 +909,11 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="8"/>
@@ -940,19 +957,19 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="8"/>
@@ -1036,7 +1053,7 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
@@ -1056,7 +1073,7 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="6"/>
@@ -1092,7 +1109,7 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
@@ -1120,7 +1137,7 @@
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="8"/>
@@ -1148,7 +1165,7 @@
       </c>
       <c r="G13">
         <f ca="1">IF(B13=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <f ca="1">IF(B13=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
@@ -1176,11 +1193,11 @@
       </c>
       <c r="N13">
         <f ca="1">IF(D13=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <f ca="1">IF(D13=1, IF(RAND()&gt;0.75, 1, 0), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>